<commit_message>
⚡️ Datos que faltaban hasta el 10
</commit_message>
<xml_diff>
--- a/aplicaciones/www/estaticos/datos/descarga/ya10-2-reclutamiento-menores.xlsx
+++ b/aplicaciones/www/estaticos/datos/descarga/ya10-2-reclutamiento-menores.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28627"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/df_mendivelso10_uniandes_edu_co/Documents/IMAGINA/Datos_Niñez_Ya/Indicadores/YA_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_60C6943C5D9FAB671D818D13F6CA5B9F33F2AC1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C79BAA2B-8AE4-4FB0-8A19-08CFF640A392}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_60C6943C5D9FAB671D818D13F6CA5B9F33F2AC1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{851B18B2-B6BC-4EF4-9E10-079771A6A3B5}"/>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="585" windowWidth="29280" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39960" yWindow="585" windowWidth="29280" windowHeight="15615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="datos" sheetId="1" r:id="rId1"/>
+    <sheet name="metadatos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>codmpio</t>
   </si>
@@ -46,18 +47,52 @@
   <si>
     <t>reclu</t>
   </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>Fecha_de_extracción</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Código del municipio</t>
+  </si>
+  <si>
+    <t>No. total de reclutamientos en niños/niñas y adolescentes en el contexto del conflicto</t>
+  </si>
+  <si>
+    <t>Panel CEDE - Registro Único de Víctimas
+Instituto Colombiano de Bienestar Familiar (ICBF)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
@@ -36589,4 +36628,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2933F5-3734-4FDC-8D1A-FC3AFDF91DC9}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45722</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>